<commit_message>
added the final version
</commit_message>
<xml_diff>
--- a/adam_smith.xlsx
+++ b/adam_smith.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="431">
   <si>
     <t xml:space="preserve">Paper </t>
   </si>
@@ -2784,6 +2784,2057 @@
   <si>
     <t xml:space="preserve">Jon Llewellyn Kyl 
 Republican Party</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, WEDNESDAY, MAY 6, 2009</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Jack Kemp was a self-taught man. He read the economic classics, beginning with </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith’s </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Wealth of Nations. He also read and studied the Declaration of Independence. Both, as it happens, were published in 1776, year 1 of our country’s independence.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Kemp taught himself by reading the economic classics beginning with </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith’s </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Wealth of Nations, but he also read and studied the Declaration of Independence, both as it happens, were, published in 1776, year one of America’s independence. Kemp mastered . . . and spelled out for us . . . the great insight that economic freedom and political freedom are intertwined and integrated parts of the order of human freedom. He reminded us that families, faith, and education—not government—are the true sources of the qualities of character without which there can be neither economic nor political freedom.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF111111"/>
+        <rFont val="Segoe UI"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Paul Davis Ryan
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Republican Party
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, TUESDAY, MAY 12, 2009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, FRIDAY, JULY 27, 2007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, THURSDAY, SEPTEMBER 6, 2007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, FRIDAY, SEPTEMBER 7, 2007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, WEDNESDAY, SEPTEMBER 19, 2007</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">The only reason to vote against this bill at this point is not because of disagreement on some of the specifics. They will evolve as we go forward, particularly in the PAYGO response. But if you believe this is something that should be left to the market, and I do not believe that the market can or should be asked to handle terrorism. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">is one of the great intellectual contributors to thought in this world, but I don’t think he knew much about terrorism, luckily for him. I do not think that the free market was adopted or is adaptable to murderous attacks of the sort we had on September 11.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Barney Frank 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF111111"/>
+        <rFont val="Segoe UI"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Democratic Party</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, TUESDAY, SEPTEMBER 25, 2007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, WEDNESDAY, OCTOBER 17, 2007</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">e, if parents take responsibility for their children’s health insurance that this invisible hand that </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">wrote about, this consumer’s guide to how the health care in America will be developed, how it will evolve, how the research will be done, how the development will be done, how we will be marketing health insurance and how we will be providing services, this best system we have in the world is something we want to preserve.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, THURSDAY, OCTOBER 18, 2007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, TUESDAY, NOVEMBER 13, 2007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, THURSDAY, NOVEMBER 15, 2007</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">There is a time for Government. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, in his great book ‘‘The Wealth of Nations,’’ in 1776, said there is a place for Government. If he were writing that book today, he would talk about the need for Government throughout America in many different ways. One thing we need to do is do something with FHA, with Fannie and Freddie, which are organizations we set up in Congress to help people buy homes</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">‘‘The Wealth of Nations,’’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, THURSDAY, DECEMBER 13, 2007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, THURSDAY, FEBRUARY 14, 2008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, FRIDAY, FEBRUARY 29, 2008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, FRIDAY, MARCH 14, 2008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, WEDNESDAY, APRIL 2, 2008</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">The reduction in industrial investment that took place January, February, March, April and onwards of 2007 was the lead indicator for this economic inactivity that we’re seeing today. That was item number one, the understanding that there would be tax increases, this understanding that we know, according to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">and Wealth of Nations from 1776 when he said ‘‘the cost of any goods is the cost of the labor that it takes to produce it and the capital required to support the labor.’’</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">- Wealth of Nations
+-‘‘the cost of any goods is the cost of the labor that it takes to produce it and the capital required to support the labor.’’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, TUESDAY, APRIL 8, 2008</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">My goodness, I think </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> would be rolling over in his grave to hear this concept of economics. This is Komisar economics where nobody can lose, except for the taxpayer in the next generation who has to pay this bill. Remember, this $20 billion is going to be paid by somebody because it is being spent around here in the operation of the Government. And who is going to pay it? Well, it is obviously not going to be the homebuilder, the large corporations which ran up these huge profits. They are actually going to take that money in, take it in as income.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Well, as I said, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">would be a little stunned to find this is the way the market has worked and the Government of the United States—which is allegedly the Government of a capitalist system—functions.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF111111"/>
+        <rFont val="Segoe UI"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">William Gregory Steube
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Republican Party</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, THURSDAY, APRIL 10, 2008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, WEDNESDAY, APRIL 23, 2008</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Then, as </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">ADAM SMITH </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">said, there are two components to the price of everything. One is the cost of the labor and the other is the cost of the capital. The capital price went up, then the cost of goods and services went up, and capital investment went down.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. And when I hear about </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">ADAM SMITH </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">being talked about, the only ‘‘invisible hand’’ that is operating in our energy markets is that invisible handshake that happened in the White House between the oil company executives when they created this current energy policy.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">And, as they invested in those countries, their profits rose, and the jobs in America, according to I guess Adam Smith, the invisible hand pulled them and grabbed them to China. And when they couldn’t do it in China anymore, they pulled them and grabbed them to Vietnam. And when they couldn’t do it in Vietnam, they pulled them to Bangladesh.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-‘‘invisible hand’’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tim Walz
+Democratic–Farmer–Labor Party (DFL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, TUESDAY, MAY 6, 2008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, THURSDAY, MAY 8, 2008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, MONDAY, MAY 19, 2008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, WEDNESDAY, MAY 21, 2008</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">As someone who voted for every free trade agreement since being elected to Congress in 1992, this section is not protectionism. Back in 1776, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">argued in his celebrated ‘‘Wealth of Nations’’; that ‘‘it is of importance that the kingdom should depend as little as possible upon its neighbors for the manufactures necessary for its defense.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF111111"/>
+        <rFont val="Segoe UI"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Donald Anthony Manzullo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Republican Party</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, THURSDAY, MAY 22, 2008</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">argued in 1776: The directors of . . . [joint-stock] companies, . . . being the managers rather of other people’s money than of their own, it cannot well be expected, that they should watch over it with the same anxious vigilance with which the partners in a private copartnery frequently watch over their own.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Daniel Kahikina Akaka
+Democratic Party</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">This farm bill runs counter to all the concepts of a free market society from which this country has benefited so dramatically and which we believe to be true and effective ways to produce product and control costs and to make product more cost-effective for the people who use it. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">was right; Karl Marx was wrong. Under this bill, one would think Karl Marx was right and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">was wrong.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">William Gregory Steube
+Republican Party</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, THURSDAY, JUNE 3, 2004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, THURSDAY, JUNE 24, 2004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, FRIDAY, JUNE 25, 2004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, TUESDAY, JULY 20, 2004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, MONDAY, SEPTEMBER 13, 2004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, FRIDAY, SEPTEMBER 24, 2004</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">He has always been a free trader, a believer in Ricardo and the doctrine of comparative advantage, and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. You know, the common sense notion that if you can produce the textiles in England—the sheep and the wool and the textiles—and you can raise the grapes in Portugal to produce the wine, it makes good sense for England to trade the textiles for the wine, and the English can drink and the Portuguese can wear wool.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Byron Dorgan
+Democratic Party</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, THURSDAY, SEPTEMBER 30, 2004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, SATURDAY, OCTOBER 9, 2004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, TUESDAY, NOVEMBER 16, 2004</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Very few come to the floor to talk about the doctrine of comparative advantage and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">and the kind of things that I have had the privilege of hearing from Senator HOLLINGS.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, WEDNESDAY, FEBRUARY 9, 2005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, THURSDAY, FEBRUARY 10, 2005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, THURSDAY, MARCH 10, 2005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, MONDAY, MAY 16, 2005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, WEDNESDAY, MAY 18, 2005</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">The intent of Congress is to maintain the vibrant industrial base so that we may remain the strongest Nation on Earth. Even the founder of modern-day capitalism and free trade, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, recognized the need for a nation to be able to depend upon its own industrial and agricultural base and not rely on foreign sources for its defense needs. We cannot maintain our role as global leader on a pure services-based economy.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, THURSDAY, MAY 19, 2005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, THURSDAY, MAY 26, 2005</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Even the founder of modern-day capitalism and free trade, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, recognized the need for a nation to be able to depend upon its own industrial and agricultural base and not rely on foreign sources for its defense needs. We cannot maintain our role as global leader on a pure services-based economy.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, THURSDAY, JUNE 5, 2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, WEDNESDAY, JUNE 18, 2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, WEDNESDAY, JUNE 25, 2003</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">My Republican colleagues, on the other hand, seem to feel that the invisible hand of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">and the hand of God are the same thing but our free market is not an all-powerful system without limitations.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Loretta Lorna Sanchez
+Democratic Party</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, WEDNESDAY, JULY 9, 2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, MONDAY, JULY 14, 2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, TUESDAY, JULY 22, 2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, THURSDAY, JULY 24, 2003</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">I would point out that </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">wrote this in about 1776, that ‘‘if you can buy it cheaper than you can make it, you ought to buy it; if you can make it cheaper than you can buy it, you ought to make it.’’ That is what this is about, this Free Trade Agreement.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, TUESDAY, SEPTEMBER 30, 2003</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">The idea of such tuition grants is not new. For almost two centuries various proposals for the idea have come from such figures as </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, Thomas Paine, John Stewart Mill, and more recently Milton Friedman. Its appeal bridges ideological differences. Yet it had never been tried. Quite possibly because the need for it has never been so demonstrably critical as now</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">John Lester Hubbard Chafee
+Republican Party</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, WEDNESDAY, OCTOBER 29, 2003</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Some adopt the rhetorical convention that criticism of China’s trade policies amounts to protectionism. But </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">himself would not have recognized China as a free market bulwark. The term that he would have used to describe China’s economic policies is mercantilistic, and mercantilism has no place in today’s global marketplace which is guided by a rules-based system where ‘‘beggar thy neighbor’’ is not part of the equation</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Xavier Becerra
+Democratic Party</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, SATURDAY, NOVEMBER 22, 2003</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">The people of Great Britain also might see some familiar traits in Americans. We’re sometimes faulted for a naive faith that liberty can change the world. If that’s an error it began with reading too much John Locke and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. Americans have, on occasion, been called moralists who often speak in terms of right and wrong. That zeal has been inspired by examples on this island, by the tireless compassion of Lord Shaftesbury, the righteous courage of Wilberforce, and the firm determination of the Royal Navy over the decades to fight and end the trade in slaves.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">PRESIDENT BUSH      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, TUESDAY, DECEMBER 9, 2003</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Free trade and free markets are essentially about making trade easier by allowing the market to balance needs, supply and demand. We are engaged in a battle to tear down trade barriers around the world in an effort to promote jobs, competition and greater prosperity for all countries involved. Since </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">explained the benefits of free trade in his great work ‘‘The Wealth of Nations’’, thoughtful policy makers have understood the need to reduce these barriers. The famous economist Joseph Schumpeter once proclaimed that capitalism relies on the free flow of information and goods</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">-‘‘The Wealth of Nations’’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tom Feeney
+Republican</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, THURSDAY, FEBRUARY 26, 2004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, THURSDAY, MARCH 11, 2004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, WEDNESDAY, MARCH 31, 2004</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">In the past, and for the last actually 150 or so years, a lot of people have been wedded to the concept of free trade as described by various economists, from Ricardo and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, and we adhere, most of us, to the concept that free trade is good in the long run and produces in fact a more viable economy. That has been the mantra many people have chanted.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Tom Tancredo
+Republican</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, TUESDAY, APRIL 27, 2004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, WEDNESDAY, APRIL 28, 2004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, THURSDAY, MAY 6, 2004</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">They would be dismayed to see how little heed has been paid to the warning of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, the founding high priest of capitalism, that without fair rules of the game to keep markets honest that capitalism could be misaligned into a system that provided insufficient protection for the legitimate interests of workers and consumers alike.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Tammy Baldwin
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF111111"/>
+        <rFont val="Segoe UI"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Democratic Party</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, TUESDAY, MAY 11, 2004</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">The American people deserve the credit for that, but there is still one anchor on the neck of the economy. The biggest drag on the neck of the economy is the IRS. 230 years ago, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">wrote that the market was the invisible hand of the economy. I agree with that. And 230 years later, we can say that the visible foot on the throat of the economy is the IRS code</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">John Elmer Linder
+Republican</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, WEDNESDAY, MAY 12, 2004</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">I remember a Congressman coming into my district in the early 1980s making a pitch for a national health care act. And I remember in that room of about 80 people, in the end I was the only one of the employers in the room that provided health insurance for my employees, and I remember fighting off that effort of going for a national health care because we need more individual responsibility so that we have more individual decisions made, in the vision of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> and the invisible hand</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, WEDNESDAY, MAY 19, 2004</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Mr. REID. Mr. President, a great book, certainly a classic, was written in 1776 by </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">called ‘‘The Wealth Of Nations.’’ This was the first time it was put down on paper that someone understood, from an economist’s point of view, what the free enterprise system was and could be, and that is the basis for our country, this free enterprise system we hear so much about, capitalism, free markets. That is, in effect, what this debate is all about</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">‘‘The Wealth Of Nations.’’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, FRIDAY, MAY 21, 2004</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Let me be extra clear about one thing: This bill will help markets for credit work better. As </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">told us, the free flow of information is an absolute prerequisite of an efficient market. For markets to work, buyers must know and understand what they are buying. When our bill becomes law, credit card holders—who are simply buyers of credit in the marketplace— will have a better understanding of what exactly they are buying into, for the long term. The result can only be that the credit markets will better serve us, and that our households and our Nation will be on stronger financial footing.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Richard Joseph Durbin
+Democratic Party</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, THURSDAY, MARCH 15, 2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, THURSDAY, MARCH 22, 2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, WEDNESDAY, MARCH 28, 2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Economists have always been interested in the economics of the arts. Adam Smith is a well-known economist. He was also a serious, but littleknown essayist on painting, dancing, and poetry. Keynes was a passionate devotee of painting.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pete V. Domenici
+Republican Party</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, THURSDAY, MARCH 29, 2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, TUESDAY, APRIL 24, 2001</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">That is a definition that can be applied to our country as we see a global market develop in all sorts of commodities. It becomes very clear that the theories of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">apply in our society and in our world today. There are certain products and certain capabilities which one society is better at than other societies. Fortunately, our society is best at those activities which produce the most wealth and the most prosperity. A large percentage of those products and capabilities involve technology. They involve intellectual capacity, and they require a strong education system to succeed.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, THURSDAY, APRIL 26, 2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, THURSDAY, MAY 10, 2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, THURSDAY, MAY 17, 2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, WEDNESDAY, OCTOBER 13, 1999</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">These arguments are no truer today than they were at the turn of the century. The current trend towards concentration in agriculture is not the product of the ‘‘free market,’’ nor of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith’s </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">invisible hand. For starters, with no effective competition in the major commodity markets, these can hardly be held up as models of free market competition. What they really stand for is market failure. In any event, these near-monopolies were not created by the free market at all. They were created by government, just like the railroad monopolies of the 19th century. Instead of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith’s </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">invisible hand, we are seeing the hand of multinational food conglomerates, in the words of Iowa farmer Jim Braun, ‘‘acting inside the glove of government.’</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Paul David Wellstone
+Democratic Party</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, WEDNESDAY, OCTOBER 27, 1999</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Go right back to Alexander Hamilton in the earliest days. In the earliest days, you had that doctrine of market forces, comparative advantage, and David Ricardo. That is what they said, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">—you go ahead, the little fledgling colony that now had won its independence, you produce best what you can and ship it back to the mother country and the mother country in turn will produce and ship back what we can produce best—the doctrine of comparative advantage.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Ernest Frederick “Fritz” Hollings
+Democratic Party</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, THURSDAY, OCTOBER 28, 1999</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Everybody knows Korea have used the Japanese system of controlled capitalism, and it works. That was the American system under Alexander Hamilton. We point out time and again to the Brits, once we won our freedom in the earliest days—David Ricardo, the doctrine of comparative advantage; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, open markets, let’s go right now. The Brits corresponded with Hamilton saying: You fledgling colony, now that you have won your freedom, let’s trade back to the mother country with what you produce best and we will trade back with you what we produce best.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, MONDAY, NOVEMBER 1, 1999</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">The other side of the aisle has been wanting to do away with all kinds of trade agreements and market forces, and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">has long since gone in this global competition. It ought to depend on market forces. They depend on protection. Of course, so does the other side of the aisle when it comes to intellectual property, movies, books, copyrighting, when it comes to protecting the talents of the individual producers, the authors, writers, singers, and performers. Fine, let’s have protection for them. But for those who work by the sweat of their brow, that is protectionism and a terrible thing. </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, TUESDAY, NOVEMBER 2, 1999</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Information technology may be giving birth, too, to an economy that is close to the theoretical models of capitalism imagined by </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">and his admirers. Those models assumed that the world was made up of rational individuals who were able to pursue their economic interests in the light of perfect information and relatively free from government and geographical obstacles. Geography is becoming less of a constraint; governments are becoming less interventionist; and information is more easily and rapidly available.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, TUESDAY, NOVEMBER 9, 1999</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">One suggestion for the date of the new holiday was June 5, for </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith’s </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">birthday. But the most votes went for Nov. 9, the day the wall fell. So today I proclaim that date Freedom Day.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Mr. Christopher Cox
+Republican Party</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">The whole purpose of this bill is to say that those who get deeply into debt should have to repay their debts, even if they are poor. I understand that. I do not agree with certain provisions of it, but I understand it. We can all agree that we ought to have full and broad disclosure before someone signs up for a credit card so they do not get mired in that debt. That is not a Democratic or Republican principle, it is an </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">free market principle: full information.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">We are simply providing information. This is good old </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> American competition, and companies will compete for people based on who has the best rates.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Chuck Schumer
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF111111"/>
+        <rFont val="Segoe UI"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Democratic Party</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, WEDNESDAY, NOVEMBER 17, 1999</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">So I withdraw my objection to this amendment. I know it is offered in good faith. But please let my colleagues understand that if you want real disclosure—no more, just disclosure, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">economics—the only way to get it is not by an amendment that allows the industry to continue deceptive practices but, rather, by the Schumer-Santorum amendment which says, in no uncertain terms, ‘‘9.99 percent’’—whatever the interest rate is— 24-point type, in large letters</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, THURSDAY, FEBRUARY 10, 2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, TUESDAY, MARCH 14, 2000</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Now, some people say, well, it is the market. Let the market work. Well, let the market, if the market works in a true market form. I am a firm believer in </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. I am a strong believer in the philosophy of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">and capitalism and the market. But it is an unfair advantage in the market if we let a cartel go in. The cartel is not a concept of the market, and that is what is happening to your gasoline prices.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">If we had a true market form the way that </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">talked about a true market, we would not have a cartel out there, competition would be allowed to thrive, and we would not have this kind of situation occurring. The administration has got to recognize they do not have an </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">type of playing field out there, they have got a cartel. And that is what is jacking up the price to the American people. The American people deserve an aggressive behavior out of its Nation’s capital before our economy begins to crumble as a result of these oil prices.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Scott McInnis
+Republican Party</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, TUESDAY, MARCH 21, 2000</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, Wealth of Nations, talked about a cartel, and the cartel, of course, as my colleagues know, is OPEC. So first of all, let us define what we are dealing with out there and then we will move on, because that helps us have a clear focus on the problem and then we can move on to what I think some of the solutions are.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">in my opinion, one of the greatest philosophers and writers about capitalism in this country, or in the history of the world was </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith. Adam Smith </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">says a cartel, he did not use the word cartel, he called it a monopoly, ‘‘A monopoly granted either to an individual or to a trading company has the same effect as a secret in trade or manufactures. The monopolists, by keeping the market constantly understocked, by never fully supplying the effectual demand, sell their commodities much above the natural price, and raise their compensation, whether they consist in wages or profit, greatly above the natural rate.’’ So we have a system in balance out there. The natural rate is what Adam Smith refers to. But the monopoly allows one to exceed the natural rate.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">We need to fund our defense. We need to fund our transportation, et cetera, et cetera. But years and years ago, because some people in this country thought that other people in this country were too wealthy and that we really ought to transfer wealth instead of through work or instead of through the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">ADAM SMITH </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">philosophy, we ought to transfer wealth by going to the wealthy people and saying we taxed you throughout your life; but upon death, we are going to go ahead and tax property that has already been taxed. That is a clever way to redistribute wealth. Let us just defy the age-old proven theory of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">ADAM SMITH </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">and the open market. Let us just transfer, redistribute wealth by taking from the rich and giving to the poor, the old Robin Hood philosophy. That is kind of the beginnings of the death tax in this country.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Wealth of Nations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, TUESDAY, APRIL 11, 2000</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">This is a transfer tax. It is a defiance of the capitalistic system. It is a tax that would have </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">turn in his grave. His Wealth of Nations has a special chapter devoted to just exactly this problem in a capitalistic system.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, THURSDAY, MAY 11, 2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, THURSDAY, MAY 18, 2000</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Generally speaking, what is going on here is that </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">is spinning in his grave. General Electric wants us to socialize the risk but privatize the profit for them. But all of the American taxpayers are going to shoulder the burden.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Edward John Markey
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF111111"/>
+        <rFont val="Segoe UI"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Democratic Party</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, THURSDAY, MAY 23, 1996</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Mr. GENE GREEN of Texas. Mr. Speaker, to my colleague from California, 1.3 million workers will see a pay increase if the minimum wage is passed. The gentleman’s quote from U.S. News and World Report is straight out of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, but it is more like the Addams Family. hhhhhhh</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Raymond Eugene “Gene” Green
+ Democratic Party</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">When wages fall, buying power drops, and all these </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">economists would then come to use and say, well, we have social problems now. So Federal Government, give us money for more police officers; Federal Government, give us more money for courts; Federal Government, give us more money to build prisons.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Ronald Paul Klink
+Democratic Party</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON, TUESDAY, MAY 23, 1995</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">As everybody knows, a little earlier this year, in part those record trade deficits led to a plummeting of the value of the United States dollar versus the yen and the German mark. The dollar has recovered a bit but still is at near post-World War II historic lows. A lot of the responsibility for this has to be put at the doorstep of those who continue to mindlessly follow a trade policy which came to maturity under the leadership of Ronald Reagan in the early 1980’s, following the dictates of an economist who has been dead for 200 years, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, a man who never saw an airplane, never even saw a steam engine. Yet this man dictates the trade policy of the United States of America. Only two countries in the world follow </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adam Smith’s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> trade theories. We are both international basket cases: the United States of America and Great Britain</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Peter Anthony DeFazio
+Democratic Party</t>
   </si>
 </sst>
 </file>
@@ -3084,7 +5135,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F152"/>
+  <dimension ref="A1:F212"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -4784,229 +6835,1177 @@
         <v>262</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="4"/>
-      <c r="B125" s="5"/>
-      <c r="C125" s="5"/>
+    <row r="125" customFormat="false" ht="36.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="B125" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="C125" s="7" t="s">
+        <v>265</v>
+      </c>
       <c r="D125" s="5"/>
       <c r="E125" s="5"/>
-      <c r="F125" s="12"/>
+      <c r="F125" s="8" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="4"/>
-      <c r="B126" s="5"/>
+      <c r="A126" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="B126" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="C126" s="5"/>
       <c r="D126" s="5"/>
       <c r="E126" s="5"/>
       <c r="F126" s="12"/>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="4"/>
-      <c r="B127" s="5"/>
+      <c r="A127" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="B127" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="C127" s="5"/>
       <c r="D127" s="5"/>
       <c r="E127" s="5"/>
       <c r="F127" s="12"/>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="4"/>
-      <c r="B128" s="5"/>
+      <c r="A128" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="B128" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="C128" s="5"/>
       <c r="D128" s="5"/>
       <c r="E128" s="5"/>
       <c r="F128" s="12"/>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="4"/>
-      <c r="B129" s="5"/>
+      <c r="A129" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="B129" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="C129" s="5"/>
       <c r="D129" s="5"/>
       <c r="E129" s="5"/>
       <c r="F129" s="12"/>
     </row>
-    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="4"/>
-      <c r="B130" s="5"/>
+    <row r="130" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="B130" s="7" t="s">
+        <v>272</v>
+      </c>
       <c r="C130" s="5"/>
       <c r="D130" s="5"/>
       <c r="E130" s="5"/>
-      <c r="F130" s="12"/>
+      <c r="F130" s="8" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="4"/>
-      <c r="B131" s="5"/>
+      <c r="A131" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="B131" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="C131" s="5"/>
       <c r="D131" s="5"/>
       <c r="E131" s="5"/>
       <c r="F131" s="12"/>
     </row>
-    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="4"/>
-      <c r="B132" s="5"/>
+    <row r="132" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="B132" s="7" t="s">
+        <v>276</v>
+      </c>
       <c r="C132" s="5"/>
       <c r="D132" s="5"/>
       <c r="E132" s="5"/>
-      <c r="F132" s="12"/>
+      <c r="F132" s="12" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="4"/>
-      <c r="B133" s="5"/>
+      <c r="A133" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="B133" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="C133" s="5"/>
       <c r="D133" s="5"/>
       <c r="E133" s="5"/>
       <c r="F133" s="12"/>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="4"/>
-      <c r="B134" s="5"/>
+      <c r="A134" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="B134" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="C134" s="5"/>
       <c r="D134" s="5"/>
       <c r="E134" s="5"/>
       <c r="F134" s="12"/>
     </row>
-    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="4"/>
-      <c r="B135" s="5"/>
+    <row r="135" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="B135" s="7" t="s">
+        <v>280</v>
+      </c>
       <c r="C135" s="5"/>
       <c r="D135" s="5"/>
-      <c r="E135" s="5"/>
-      <c r="F135" s="12"/>
+      <c r="E135" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="F135" s="12" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="4"/>
-      <c r="B136" s="5"/>
+      <c r="A136" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="B136" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="C136" s="5"/>
       <c r="D136" s="5"/>
       <c r="E136" s="5"/>
       <c r="F136" s="12"/>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="4"/>
-      <c r="B137" s="5"/>
+      <c r="A137" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="B137" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="C137" s="5"/>
       <c r="D137" s="5"/>
       <c r="E137" s="5"/>
       <c r="F137" s="12"/>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="4"/>
-      <c r="B138" s="5"/>
+      <c r="A138" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="B138" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="C138" s="5"/>
       <c r="D138" s="5"/>
       <c r="E138" s="5"/>
       <c r="F138" s="12"/>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="4"/>
-      <c r="B139" s="5"/>
+      <c r="A139" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="B139" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="C139" s="5"/>
       <c r="D139" s="5"/>
       <c r="E139" s="5"/>
       <c r="F139" s="12"/>
     </row>
-    <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="4"/>
-      <c r="B140" s="5"/>
+    <row r="140" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="B140" s="7" t="s">
+        <v>287</v>
+      </c>
       <c r="C140" s="5"/>
       <c r="D140" s="5"/>
-      <c r="E140" s="5"/>
-      <c r="F140" s="12"/>
-    </row>
-    <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="4"/>
-      <c r="B141" s="5"/>
-      <c r="C141" s="5"/>
+      <c r="E140" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="F140" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="B141" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="C141" s="7" t="s">
+        <v>291</v>
+      </c>
       <c r="D141" s="5"/>
       <c r="E141" s="5"/>
-      <c r="F141" s="12"/>
+      <c r="F141" s="8" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="4"/>
-      <c r="B142" s="5"/>
+      <c r="A142" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B142" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="C142" s="5"/>
       <c r="D142" s="5"/>
       <c r="E142" s="5"/>
       <c r="F142" s="12"/>
     </row>
-    <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="4"/>
-      <c r="B143" s="5"/>
+    <row r="143" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B143" s="7" t="s">
+        <v>295</v>
+      </c>
       <c r="C143" s="5"/>
       <c r="D143" s="5"/>
       <c r="E143" s="5"/>
-      <c r="F143" s="12"/>
-    </row>
-    <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="4"/>
-      <c r="B144" s="5"/>
-      <c r="C144" s="5"/>
+      <c r="F143" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B144" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C144" s="5" t="s">
+        <v>297</v>
+      </c>
       <c r="D144" s="5"/>
-      <c r="E144" s="5"/>
-      <c r="F144" s="12"/>
+      <c r="E144" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="F144" s="12" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="4"/>
-      <c r="B145" s="5"/>
+      <c r="A145" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="B145" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="C145" s="5"/>
       <c r="D145" s="5"/>
       <c r="E145" s="5"/>
       <c r="F145" s="12"/>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="4"/>
-      <c r="B146" s="5"/>
+      <c r="A146" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B146" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="C146" s="5"/>
       <c r="D146" s="5"/>
       <c r="E146" s="5"/>
       <c r="F146" s="12"/>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="4"/>
-      <c r="B147" s="5"/>
+      <c r="A147" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B147" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="C147" s="5"/>
       <c r="D147" s="5"/>
       <c r="E147" s="5"/>
       <c r="F147" s="12"/>
     </row>
-    <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="4"/>
-      <c r="B148" s="5"/>
+    <row r="148" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B148" s="7" t="s">
+        <v>304</v>
+      </c>
       <c r="C148" s="5"/>
       <c r="D148" s="5"/>
-      <c r="E148" s="5"/>
-      <c r="F148" s="12"/>
-    </row>
-    <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="4"/>
-      <c r="B149" s="5"/>
+      <c r="E148" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F148" s="13" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="B149" s="16" t="s">
+        <v>307</v>
+      </c>
       <c r="C149" s="5"/>
       <c r="D149" s="5"/>
       <c r="E149" s="5"/>
-      <c r="F149" s="12"/>
-    </row>
-    <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="4"/>
-      <c r="B150" s="5"/>
+      <c r="F149" s="12" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="B150" s="7" t="s">
+        <v>309</v>
+      </c>
       <c r="C150" s="5"/>
       <c r="D150" s="5"/>
       <c r="E150" s="5"/>
-      <c r="F150" s="12"/>
+      <c r="F150" s="12" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="4"/>
-      <c r="B151" s="5"/>
+      <c r="A151" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="B151" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="C151" s="5"/>
       <c r="D151" s="5"/>
       <c r="E151" s="5"/>
       <c r="F151" s="12"/>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="4"/>
-      <c r="B152" s="5"/>
+      <c r="A152" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B152" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="C152" s="5"/>
       <c r="D152" s="5"/>
       <c r="E152" s="5"/>
       <c r="F152" s="12"/>
+    </row>
+    <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="B153" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C153" s="5"/>
+      <c r="D153" s="5"/>
+      <c r="E153" s="5"/>
+      <c r="F153" s="12"/>
+    </row>
+    <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="B154" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C154" s="5"/>
+      <c r="D154" s="5"/>
+      <c r="E154" s="5"/>
+      <c r="F154" s="12"/>
+    </row>
+    <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="B155" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C155" s="5"/>
+      <c r="D155" s="5"/>
+      <c r="E155" s="5"/>
+      <c r="F155" s="12"/>
+    </row>
+    <row r="156" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="B156" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="C156" s="5"/>
+      <c r="D156" s="5"/>
+      <c r="E156" s="5"/>
+      <c r="F156" s="12" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="B157" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C157" s="5"/>
+      <c r="D157" s="5"/>
+      <c r="E157" s="5"/>
+      <c r="F157" s="12"/>
+    </row>
+    <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="B158" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C158" s="5"/>
+      <c r="D158" s="5"/>
+      <c r="E158" s="5"/>
+      <c r="F158" s="12"/>
+    </row>
+    <row r="159" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="B159" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="C159" s="5"/>
+      <c r="D159" s="5"/>
+      <c r="E159" s="5"/>
+      <c r="F159" s="12" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="B160" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C160" s="5"/>
+      <c r="D160" s="5"/>
+      <c r="E160" s="5"/>
+      <c r="F160" s="12"/>
+    </row>
+    <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="B161" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C161" s="5"/>
+      <c r="D161" s="5"/>
+      <c r="E161" s="5"/>
+      <c r="F161" s="12"/>
+    </row>
+    <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="B162" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C162" s="5"/>
+      <c r="D162" s="5"/>
+      <c r="E162" s="5"/>
+      <c r="F162" s="12"/>
+    </row>
+    <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="B163" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C163" s="5"/>
+      <c r="D163" s="5"/>
+      <c r="E163" s="5"/>
+      <c r="F163" s="12"/>
+    </row>
+    <row r="164" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="B164" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="C164" s="5"/>
+      <c r="D164" s="5"/>
+      <c r="E164" s="5"/>
+      <c r="F164" s="12" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="B165" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C165" s="5"/>
+      <c r="D165" s="5"/>
+      <c r="E165" s="5"/>
+      <c r="F165" s="12"/>
+    </row>
+    <row r="166" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="B166" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="C166" s="5"/>
+      <c r="D166" s="5"/>
+      <c r="E166" s="5"/>
+      <c r="F166" s="12" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="B167" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C167" s="5"/>
+      <c r="D167" s="5"/>
+      <c r="E167" s="5"/>
+      <c r="F167" s="12"/>
+    </row>
+    <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="B168" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C168" s="5"/>
+      <c r="D168" s="5"/>
+      <c r="E168" s="5"/>
+      <c r="F168" s="12"/>
+    </row>
+    <row r="169" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="B169" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="C169" s="5"/>
+      <c r="D169" s="5"/>
+      <c r="E169" s="5"/>
+      <c r="F169" s="12" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="B170" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C170" s="5"/>
+      <c r="D170" s="5"/>
+      <c r="E170" s="5"/>
+      <c r="F170" s="12"/>
+    </row>
+    <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="B171" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C171" s="5"/>
+      <c r="D171" s="5"/>
+      <c r="E171" s="5"/>
+      <c r="F171" s="12"/>
+    </row>
+    <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="B172" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C172" s="5"/>
+      <c r="D172" s="5"/>
+      <c r="E172" s="5"/>
+      <c r="F172" s="12"/>
+    </row>
+    <row r="173" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B173" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="C173" s="5"/>
+      <c r="D173" s="5"/>
+      <c r="E173" s="5"/>
+      <c r="F173" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="B174" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="C174" s="5"/>
+      <c r="D174" s="5"/>
+      <c r="E174" s="5"/>
+      <c r="F174" s="12" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="B175" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="C175" s="5"/>
+      <c r="D175" s="5"/>
+      <c r="E175" s="5"/>
+      <c r="F175" s="12" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="B176" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="C176" s="5"/>
+      <c r="D176" s="5"/>
+      <c r="E176" s="5"/>
+      <c r="F176" s="5" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="B177" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="C177" s="5"/>
+      <c r="D177" s="5"/>
+      <c r="E177" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="F177" s="12" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="B178" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C178" s="5"/>
+      <c r="D178" s="5"/>
+      <c r="E178" s="5"/>
+      <c r="F178" s="12"/>
+    </row>
+    <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="B179" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C179" s="5"/>
+      <c r="D179" s="5"/>
+      <c r="E179" s="5"/>
+      <c r="F179" s="12"/>
+    </row>
+    <row r="180" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="B180" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="C180" s="5"/>
+      <c r="D180" s="5"/>
+      <c r="E180" s="5"/>
+      <c r="F180" s="12" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="B181" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C181" s="5"/>
+      <c r="D181" s="5"/>
+      <c r="E181" s="5"/>
+      <c r="F181" s="12"/>
+    </row>
+    <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="B182" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C182" s="5"/>
+      <c r="D182" s="5"/>
+      <c r="E182" s="5"/>
+      <c r="F182" s="12"/>
+    </row>
+    <row r="183" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="B183" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="C183" s="5"/>
+      <c r="D183" s="5"/>
+      <c r="E183" s="5"/>
+      <c r="F183" s="8" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="B184" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="C184" s="5"/>
+      <c r="D184" s="5"/>
+      <c r="E184" s="5"/>
+      <c r="F184" s="12" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="B185" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="C185" s="5"/>
+      <c r="D185" s="5"/>
+      <c r="E185" s="5"/>
+      <c r="F185" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="B186" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="C186" s="5"/>
+      <c r="D186" s="5"/>
+      <c r="E186" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="F186" s="12" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="B187" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="C187" s="5"/>
+      <c r="D187" s="5"/>
+      <c r="E187" s="5"/>
+      <c r="F187" s="12" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="B188" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C188" s="5"/>
+      <c r="D188" s="5"/>
+      <c r="E188" s="5"/>
+      <c r="F188" s="12"/>
+    </row>
+    <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="B189" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C189" s="5"/>
+      <c r="D189" s="5"/>
+      <c r="E189" s="5"/>
+      <c r="F189" s="12"/>
+    </row>
+    <row r="190" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="B190" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="C190" s="5"/>
+      <c r="D190" s="5"/>
+      <c r="E190" s="5"/>
+      <c r="F190" s="12" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="B191" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C191" s="5"/>
+      <c r="D191" s="5"/>
+      <c r="E191" s="5"/>
+      <c r="F191" s="12"/>
+    </row>
+    <row r="192" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="B192" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="C192" s="5"/>
+      <c r="D192" s="5"/>
+      <c r="E192" s="5"/>
+      <c r="F192" s="12" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="B193" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C193" s="5"/>
+      <c r="D193" s="5"/>
+      <c r="E193" s="5"/>
+      <c r="F193" s="12"/>
+    </row>
+    <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="B194" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C194" s="5"/>
+      <c r="D194" s="5"/>
+      <c r="E194" s="5"/>
+      <c r="F194" s="12"/>
+    </row>
+    <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="B195" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C195" s="5"/>
+      <c r="D195" s="5"/>
+      <c r="E195" s="5"/>
+      <c r="F195" s="12"/>
+    </row>
+    <row r="196" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="B196" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="C196" s="5"/>
+      <c r="D196" s="5"/>
+      <c r="E196" s="5"/>
+      <c r="F196" s="12" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="B197" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="C197" s="5"/>
+      <c r="D197" s="5"/>
+      <c r="E197" s="5"/>
+      <c r="F197" s="12" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="B198" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="C198" s="5"/>
+      <c r="D198" s="5"/>
+      <c r="E198" s="5"/>
+      <c r="F198" s="12" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="B199" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="C199" s="5"/>
+      <c r="D199" s="5"/>
+      <c r="E199" s="5"/>
+      <c r="F199" s="12" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="B200" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="C200" s="5"/>
+      <c r="D200" s="5"/>
+      <c r="E200" s="5"/>
+      <c r="F200" s="12" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="B201" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="C201" s="5"/>
+      <c r="D201" s="5"/>
+      <c r="E201" s="5"/>
+      <c r="F201" s="12" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="202" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="B202" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="C202" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="D202" s="5"/>
+      <c r="E202" s="5"/>
+      <c r="F202" s="8" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="203" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="B203" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="C203" s="5"/>
+      <c r="D203" s="5"/>
+      <c r="E203" s="5"/>
+      <c r="F203" s="8" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="B204" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C204" s="5"/>
+      <c r="D204" s="5"/>
+      <c r="E204" s="5"/>
+      <c r="F204" s="12"/>
+    </row>
+    <row r="205" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="B205" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="C205" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="D205" s="5"/>
+      <c r="E205" s="5"/>
+      <c r="F205" s="12" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="206" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="B206" s="16" t="s">
+        <v>413</v>
+      </c>
+      <c r="C206" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="D206" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="E206" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="F206" s="12" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="207" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="B207" s="7" t="s">
+        <v>418</v>
+      </c>
+      <c r="C207" s="5"/>
+      <c r="D207" s="5"/>
+      <c r="E207" s="5"/>
+      <c r="F207" s="12" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="B208" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C208" s="5"/>
+      <c r="D208" s="5"/>
+      <c r="E208" s="5"/>
+      <c r="F208" s="12"/>
+    </row>
+    <row r="209" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="B209" s="7" t="s">
+        <v>421</v>
+      </c>
+      <c r="C209" s="5"/>
+      <c r="D209" s="5"/>
+      <c r="E209" s="5"/>
+      <c r="F209" s="8" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="210" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="B210" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="C210" s="5"/>
+      <c r="D210" s="5"/>
+      <c r="E210" s="5"/>
+      <c r="F210" s="12" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="211" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A211" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="B211" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="C211" s="5"/>
+      <c r="D211" s="5"/>
+      <c r="E211" s="5"/>
+      <c r="F211" s="12" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="212" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="4" t="s">
+        <v>428</v>
+      </c>
+      <c r="B212" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="C212" s="5"/>
+      <c r="D212" s="5"/>
+      <c r="E212" s="5"/>
+      <c r="F212" s="12" t="s">
+        <v>430</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
added file with hhhh deleted
</commit_message>
<xml_diff>
--- a/adam_smith.xlsx
+++ b/adam_smith.xlsx
@@ -68,6 +68,7 @@
         <color rgb="FF111111"/>
         <rFont val="Segoe UI"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Alvin H. Perlmutter</t>
     </r>
@@ -109,6 +110,7 @@
         <sz val="11"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">That is what capitalism is based on. That is what ADAM SMITH really wrote about.</t>
     </r>
@@ -129,6 +131,7 @@
         <sz val="11"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">the invisible hand of competitive entrepreneurship is key</t>
     </r>
@@ -151,6 +154,7 @@
         <sz val="11"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Amy Klobuchar</t>
     </r>
@@ -169,6 +173,7 @@
         <sz val="11"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Democratic Party</t>
     </r>
@@ -244,6 +249,7 @@
         <sz val="11"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">capitalist system
 </t>
@@ -265,6 +271,7 @@
         <color rgb="FF111111"/>
         <rFont val="Segoe UI"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Cory Anthony Booker</t>
     </r>
@@ -357,6 +364,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -376,6 +384,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">externalities that have to be captured, and it is government’s job to at least make sure they are captured.</t>
     </r>
@@ -407,6 +416,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith is smiling in his grave, looking at this competition unfold. </t>
     </r>
@@ -443,6 +453,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -472,6 +483,7 @@
         <sz val="11"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">free market capitalism
 </t>
@@ -493,6 +505,7 @@
         <color rgb="FF111111"/>
         <rFont val="Segoe UI"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Mike Rounds</t>
     </r>
@@ -544,6 +557,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith</t>
     </r>
@@ -588,6 +602,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -629,6 +644,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith</t>
     </r>
@@ -649,6 +665,7 @@
         <color rgb="FF111111"/>
         <rFont val="Segoe UI"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">John Cornyn</t>
     </r>
@@ -682,6 +699,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -711,6 +729,7 @@
         <sz val="11"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">capitalism. 
 </t>
@@ -748,6 +767,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith’s </t>
     </r>
@@ -766,6 +786,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith</t>
     </r>
@@ -795,6 +816,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith</t>
     </r>
@@ -897,6 +919,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -920,6 +943,7 @@
         <color rgb="FF111111"/>
         <rFont val="Segoe UI"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Kevin John Cramer</t>
     </r>
@@ -992,6 +1016,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -1024,6 +1049,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith</t>
     </r>
@@ -1066,6 +1092,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -1094,6 +1121,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith</t>
     </r>
@@ -1103,6 +1131,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -1132,6 +1161,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smit</t>
     </r>
@@ -1164,6 +1194,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith</t>
     </r>
@@ -1200,6 +1231,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -1248,6 +1280,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith</t>
     </r>
@@ -1268,6 +1301,7 @@
         <color rgb="FF111111"/>
         <rFont val="Segoe UI"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Daniel Benjamin Maffei</t>
     </r>
@@ -1301,6 +1335,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -1319,6 +1354,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -1348,6 +1384,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -1366,6 +1403,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith’s </t>
     </r>
@@ -1398,6 +1436,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith</t>
     </r>
@@ -1421,6 +1460,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smithian </t>
     </r>
@@ -1453,6 +1493,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith’s </t>
     </r>
@@ -1471,6 +1512,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -1500,6 +1542,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -1538,6 +1581,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith.</t>
     </r>
@@ -1565,6 +1609,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">, Adam Smith</t>
     </r>
@@ -1607,6 +1652,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ADAM SMITH </t>
     </r>
@@ -1625,6 +1671,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ADAM SMITH</t>
     </r>
@@ -1654,6 +1701,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith</t>
     </r>
@@ -1672,6 +1720,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -1713,6 +1762,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith</t>
     </r>
@@ -1745,6 +1795,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -1777,6 +1828,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith</t>
     </r>
@@ -1809,6 +1861,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith. This is Adam Smith </t>
     </r>
@@ -1838,6 +1891,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith’s vision, Adam Smith’s </t>
     </r>
@@ -1870,6 +1924,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -1902,6 +1957,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -1949,6 +2005,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -1979,6 +2036,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -2015,6 +2073,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith’s </t>
     </r>
@@ -2045,6 +2104,7 @@
         <color rgb="FF111111"/>
         <rFont val="Segoe UI"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Democratic Party</t>
     </r>
@@ -2065,6 +2125,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith, </t>
     </r>
@@ -2105,6 +2166,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith’s</t>
     </r>
@@ -2141,6 +2203,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -2180,6 +2243,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith</t>
     </r>
@@ -2216,6 +2280,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -2248,6 +2313,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith</t>
     </r>
@@ -2268,6 +2334,7 @@
         <color rgb="FF111111"/>
         <rFont val="Segoe UI"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -2301,6 +2368,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith</t>
     </r>
@@ -2330,6 +2398,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -2362,6 +2431,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith’s </t>
     </r>
@@ -2403,6 +2473,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -2439,6 +2510,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -2457,6 +2529,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith</t>
     </r>
@@ -2483,6 +2556,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith</t>
     </r>
@@ -2513,6 +2587,7 @@
         <color rgb="FF111111"/>
         <rFont val="Segoe UI"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Republican Party</t>
     </r>
@@ -2542,6 +2617,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -2571,6 +2647,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -2589,6 +2666,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith</t>
     </r>
@@ -2624,6 +2702,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -2656,6 +2735,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -2674,6 +2754,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith</t>
     </r>
@@ -2715,6 +2796,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith’s </t>
     </r>
@@ -2745,6 +2827,7 @@
         <color rgb="FF111111"/>
         <rFont val="Segoe UI"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Republican Party</t>
     </r>
@@ -2768,6 +2851,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith’s </t>
     </r>
@@ -2804,6 +2888,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith’s </t>
     </r>
@@ -2833,6 +2918,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith’s </t>
     </r>
@@ -2862,6 +2948,7 @@
         <color rgb="FF111111"/>
         <rFont val="Segoe UI"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Paul Davis Ryan
 </t>
@@ -2908,6 +2995,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -2938,6 +3026,7 @@
         <color rgb="FF111111"/>
         <rFont val="Segoe UI"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Democratic Party</t>
     </r>
@@ -2973,6 +3062,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -3011,6 +3101,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith</t>
     </r>
@@ -3058,6 +3149,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -3094,6 +3186,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith</t>
     </r>
@@ -3123,6 +3216,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -3152,6 +3246,7 @@
         <color rgb="FF111111"/>
         <rFont val="Segoe UI"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">William Gregory Steube
 </t>
@@ -3188,6 +3283,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ADAM SMITH </t>
     </r>
@@ -3217,6 +3313,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ADAM SMITH </t>
     </r>
@@ -3268,6 +3365,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -3288,6 +3386,7 @@
         <color rgb="FF111111"/>
         <rFont val="Segoe UI"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Donald Anthony Manzullo</t>
     </r>
@@ -3312,6 +3411,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -3345,6 +3445,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -3363,6 +3464,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -3414,6 +3516,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith</t>
     </r>
@@ -3456,6 +3559,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -3500,6 +3604,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith</t>
     </r>
@@ -3535,6 +3640,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith</t>
     </r>
@@ -3573,6 +3679,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -3618,6 +3725,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -3650,6 +3758,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith</t>
     </r>
@@ -3686,6 +3795,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -3722,6 +3832,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith</t>
     </r>
@@ -3757,6 +3868,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -3802,6 +3914,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith</t>
     </r>
@@ -3844,6 +3957,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith</t>
     </r>
@@ -3874,6 +3988,7 @@
         <color rgb="FF111111"/>
         <rFont val="Segoe UI"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Democratic Party</t>
     </r>
@@ -3906,6 +4021,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -3942,6 +4058,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith</t>
     </r>
@@ -3974,6 +4091,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -4009,6 +4127,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -4064,6 +4183,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -4105,6 +4225,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith’s </t>
     </r>
@@ -4123,6 +4244,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith’s </t>
     </r>
@@ -4159,6 +4281,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith</t>
     </r>
@@ -4195,6 +4318,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith</t>
     </r>
@@ -4227,6 +4351,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -4259,6 +4384,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -4291,6 +4417,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith’s </t>
     </r>
@@ -4324,6 +4451,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -4353,6 +4481,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith</t>
     </r>
@@ -4383,6 +4512,7 @@
         <color rgb="FF111111"/>
         <rFont val="Segoe UI"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Democratic Party</t>
     </r>
@@ -4406,6 +4536,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -4441,6 +4572,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith</t>
     </r>
@@ -4459,6 +4591,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -4488,6 +4621,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -4506,6 +4640,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -4533,6 +4668,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith</t>
     </r>
@@ -4562,6 +4698,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith. Adam Smith </t>
     </r>
@@ -4591,6 +4728,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ADAM SMITH </t>
     </r>
@@ -4609,6 +4747,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ADAM SMITH </t>
     </r>
@@ -4644,6 +4783,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -4679,6 +4819,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -4709,6 +4850,7 @@
         <color rgb="FF111111"/>
         <rFont val="Segoe UI"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Democratic Party</t>
     </r>
@@ -4732,6 +4874,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith</t>
     </r>
@@ -4742,7 +4885,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">, but it is more like the Addams Family. hhhhhhh</t>
+      <t xml:space="preserve">, but it is more like the Addams Family.</t>
     </r>
   </si>
   <si>
@@ -4765,6 +4908,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith </t>
     </r>
@@ -4801,6 +4945,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith</t>
     </r>
@@ -4819,6 +4964,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam Smith’s</t>
     </r>
@@ -4904,12 +5050,14 @@
       <color rgb="FF111111"/>
       <name val="Segoe UI"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -4923,6 +5071,7 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -4930,6 +5079,7 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -5137,11 +5287,11 @@
   </sheetPr>
   <dimension ref="A1:F212"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A65" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F78" activeCellId="0" sqref="F78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -7965,7 +8115,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="210" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="210" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="4" t="s">
         <v>423</v>
       </c>

</xml_diff>